<commit_message>
Vector database + Cosin
</commit_message>
<xml_diff>
--- a/profile_matches.xlsx
+++ b/profile_matches.xlsx
@@ -533,13 +533,13 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>(570, 988)</t>
+          <t>£570-£988</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.632</v>
+        <v>0.63</v>
       </c>
       <c r="B3" t="n">
         <v>309</v>
@@ -580,13 +580,13 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>(586, 957)</t>
+          <t>£586-£957</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.6196000000000002</v>
+        <v>0.62</v>
       </c>
       <c r="B4" t="n">
         <v>265</v>
@@ -631,13 +631,13 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>(523, 824)</t>
+          <t>£523-£824</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.6095000000000002</v>
+        <v>0.61</v>
       </c>
       <c r="B5" t="n">
         <v>209</v>
@@ -682,13 +682,13 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>(530, 855)</t>
+          <t>£530-£855</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.5927</v>
+        <v>0.59</v>
       </c>
       <c r="B6" t="n">
         <v>14</v>
@@ -725,13 +725,13 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
         <is>
-          <t>(657, 840)</t>
+          <t>£657-£840</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.588</v>
+        <v>0.59</v>
       </c>
       <c r="B7" t="n">
         <v>40</v>
@@ -768,13 +768,13 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>(532, 980)</t>
+          <t>£532-£980</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.5780000000000001</v>
+        <v>0.58</v>
       </c>
       <c r="B8" t="n">
         <v>133</v>
@@ -811,13 +811,13 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>(543, 917)</t>
+          <t>£543-£917</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.5683</v>
+        <v>0.57</v>
       </c>
       <c r="B9" t="n">
         <v>13</v>
@@ -862,13 +862,13 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>(644, 851)</t>
+          <t>£644-£851</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.5528000000000001</v>
+        <v>0.55</v>
       </c>
       <c r="B10" t="n">
         <v>389</v>
@@ -909,7 +909,7 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr">
         <is>
-          <t>(628, 959)</t>
+          <t>£628-£959</t>
         </is>
       </c>
     </row>
@@ -960,13 +960,13 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>(572, 961)</t>
+          <t>£572-£961</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.5302</v>
+        <v>0.53</v>
       </c>
       <c r="B12" t="n">
         <v>434</v>
@@ -1007,13 +1007,13 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>(691, 889)</t>
+          <t>£691-£889</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.5180000000000001</v>
+        <v>0.52</v>
       </c>
       <c r="B13" t="n">
         <v>269</v>
@@ -1050,13 +1050,13 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>(587, 900)</t>
+          <t>£587-£900</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.5092000000000001</v>
+        <v>0.51</v>
       </c>
       <c r="B14" t="n">
         <v>131</v>
@@ -1101,13 +1101,13 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>(522, 808)</t>
+          <t>£522-£808</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.4968</v>
+        <v>0.5</v>
       </c>
       <c r="B15" t="n">
         <v>462</v>
@@ -1152,13 +1152,13 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>(643, 775)</t>
+          <t>£643-£775</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.4918000000000001</v>
+        <v>0.49</v>
       </c>
       <c r="B16" t="n">
         <v>57</v>
@@ -1203,13 +1203,13 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>(570, 782)</t>
+          <t>£570-£782</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.4913</v>
+        <v>0.49</v>
       </c>
       <c r="B17" t="n">
         <v>242</v>
@@ -1254,7 +1254,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>(532, 737)</t>
+          <t>£532-£737</t>
         </is>
       </c>
     </row>
@@ -1301,13 +1301,13 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>(534, 976)</t>
+          <t>£534-£976</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.4802</v>
+        <v>0.48</v>
       </c>
       <c r="B19" t="n">
         <v>243</v>
@@ -1352,13 +1352,13 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>(524, 758)</t>
+          <t>£524-£758</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.4716</v>
+        <v>0.47</v>
       </c>
       <c r="B20" t="n">
         <v>157</v>
@@ -1403,13 +1403,13 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>(591, 824)</t>
+          <t>£591-£824</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.4691000000000001</v>
+        <v>0.47</v>
       </c>
       <c r="B21" t="n">
         <v>166</v>
@@ -1450,13 +1450,13 @@
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr">
         <is>
-          <t>(621, 910)</t>
+          <t>£621-£910</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.4651</v>
+        <v>0.47</v>
       </c>
       <c r="B22" t="n">
         <v>386</v>
@@ -1497,13 +1497,13 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>(661, 820)</t>
+          <t>£661-£820</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.426</v>
+        <v>0.43</v>
       </c>
       <c r="B23" t="n">
         <v>229</v>
@@ -1544,13 +1544,13 @@
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr">
         <is>
-          <t>(520, 840)</t>
+          <t>£520-£840</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.3878</v>
+        <v>0.39</v>
       </c>
       <c r="B24" t="n">
         <v>100</v>
@@ -1591,13 +1591,13 @@
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr">
         <is>
-          <t>(571, 722)</t>
+          <t>£571-£722</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.3782</v>
+        <v>0.38</v>
       </c>
       <c r="B25" t="n">
         <v>340</v>
@@ -1630,13 +1630,13 @@
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr">
         <is>
-          <t>(503, 778)</t>
+          <t>£503-£778</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.3759000000000001</v>
+        <v>0.38</v>
       </c>
       <c r="B26" t="n">
         <v>262</v>
@@ -1673,13 +1673,13 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>(669, 970)</t>
+          <t>£669-£970</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.3703</v>
+        <v>0.37</v>
       </c>
       <c r="B27" t="n">
         <v>155</v>
@@ -1720,13 +1720,13 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>(633, 943)</t>
+          <t>£633-£943</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.3357000000000001</v>
+        <v>0.34</v>
       </c>
       <c r="B28" t="n">
         <v>118</v>
@@ -1763,13 +1763,13 @@
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr">
         <is>
-          <t>(552, 753)</t>
+          <t>£552-£753</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.3333</v>
+        <v>0.33</v>
       </c>
       <c r="B29" t="n">
         <v>75</v>
@@ -1810,13 +1810,13 @@
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr">
         <is>
-          <t>(663, 942)</t>
+          <t>£663-£942</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.3328</v>
+        <v>0.33</v>
       </c>
       <c r="B30" t="n">
         <v>377</v>
@@ -1861,13 +1861,13 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>(608, 924)</t>
+          <t>£608-£924</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.3323</v>
+        <v>0.33</v>
       </c>
       <c r="B31" t="n">
         <v>7</v>
@@ -1908,13 +1908,13 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>(576, 727)</t>
+          <t>£576-£727</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.3312</v>
+        <v>0.33</v>
       </c>
       <c r="B32" t="n">
         <v>495</v>
@@ -1959,13 +1959,13 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>(568, 768)</t>
+          <t>£568-£768</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.3286</v>
+        <v>0.33</v>
       </c>
       <c r="B33" t="n">
         <v>217</v>
@@ -2002,13 +2002,13 @@
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr">
         <is>
-          <t>(523, 854)</t>
+          <t>£523-£854</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.3228</v>
+        <v>0.32</v>
       </c>
       <c r="B34" t="n">
         <v>489</v>
@@ -2053,13 +2053,13 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>(558, 892)</t>
+          <t>£558-£892</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.3035</v>
+        <v>0.3</v>
       </c>
       <c r="B35" t="n">
         <v>406</v>
@@ -2096,13 +2096,13 @@
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr">
         <is>
-          <t>(611, 826)</t>
+          <t>£611-£826</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.2846</v>
+        <v>0.28</v>
       </c>
       <c r="B36" t="n">
         <v>321</v>
@@ -2147,13 +2147,13 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>(580, 794)</t>
+          <t>£580-£794</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.2828</v>
+        <v>0.28</v>
       </c>
       <c r="B37" t="n">
         <v>101</v>
@@ -2190,13 +2190,13 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>(567, 792)</t>
+          <t>£567-£792</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.2576</v>
+        <v>0.26</v>
       </c>
       <c r="B38" t="n">
         <v>6</v>
@@ -2233,13 +2233,13 @@
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="inlineStr">
         <is>
-          <t>(612, 776)</t>
+          <t>£612-£776</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.2063</v>
+        <v>0.21</v>
       </c>
       <c r="B39" t="n">
         <v>44</v>
@@ -2284,13 +2284,13 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>(588, 707)</t>
+          <t>£588-£707</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.1359</v>
+        <v>0.14</v>
       </c>
       <c r="B40" t="n">
         <v>67</v>
@@ -2331,13 +2331,13 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>(512, 751)</t>
+          <t>£512-£751</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0.1332</v>
+        <v>0.13</v>
       </c>
       <c r="B41" t="n">
         <v>125</v>
@@ -2374,13 +2374,13 @@
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="inlineStr">
         <is>
-          <t>(618, 766)</t>
+          <t>£618-£766</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0.0927</v>
+        <v>0.09</v>
       </c>
       <c r="B42" t="n">
         <v>149</v>
@@ -2417,7 +2417,7 @@
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr">
         <is>
-          <t>(679, 782)</t>
+          <t>£679-£782</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
compatibility scores update after 5 likes
</commit_message>
<xml_diff>
--- a/profile_matches.xlsx
+++ b/profile_matches.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,60 +436,70 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Score</t>
+          <t>Initial Score</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Updated Score</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Score Change</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Profile ID</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Age</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Origin Country</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Occupation</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Work Industry</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Course</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Activity Hours</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Smoking</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Rent Budget</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>University</t>
         </is>
@@ -500,44 +510,50 @@
         <v>0.95</v>
       </c>
       <c r="B2" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D2" t="n">
         <v>273</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>John Doe</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="F2" t="n">
         <v>18</v>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>UK</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
         <is>
           <t>Computer Science</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>Night</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
         <is>
           <t>£901-£1054</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>UCL</t>
         </is>
@@ -545,51 +561,57 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.92</v>
       </c>
       <c r="B3" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D3" t="n">
         <v>458</v>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>Jane Johnson</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>19</v>
-      </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>USA</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr">
         <is>
           <t>Computer Science</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>Morning</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>£490-£1146</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>UCL</t>
         </is>
@@ -600,44 +622,50 @@
         <v>0.86</v>
       </c>
       <c r="B4" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D4" t="n">
         <v>276</v>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>Bob Smith</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="F4" t="n">
         <v>18</v>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>USA</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
         <is>
           <t>Computer Science</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>Night</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
         <is>
           <t>£373-£912</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>UCL</t>
         </is>
@@ -648,44 +676,50 @@
         <v>0.83</v>
       </c>
       <c r="B5" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="D5" t="n">
         <v>95</v>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Jane Doe</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="F5" t="n">
         <v>19</v>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>UK</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
         <is>
           <t>Engineering</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>Morning</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr">
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
         <is>
           <t>£303-£1987</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>UCL</t>
         </is>
@@ -696,48 +730,54 @@
         <v>0.8100000000000001</v>
       </c>
       <c r="B6" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
         <v>327</v>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>Bob Smith</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="F6" t="n">
         <v>19</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
         <is>
           <t>Computer Science</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>Morning</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="M6" t="inlineStr">
         <is>
           <t>£392-£1895</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="N6" t="inlineStr">
         <is>
           <t>City</t>
         </is>
@@ -745,47 +785,53 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.59</v>
+        <v>0.57</v>
       </c>
       <c r="B7" t="n">
-        <v>414</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Alice Johnson</t>
-        </is>
+        <v>0.63</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.06</v>
       </c>
       <c r="D7" t="n">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>UK</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Student</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr"/>
+          <t>Alice Smith</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>18</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Computer Science</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Morning</t>
-        </is>
-      </c>
+          <t>Cruising</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
-          <t>£631-£782</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>£959-£1181</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
         <is>
           <t>UCL</t>
         </is>
@@ -796,44 +842,50 @@
         <v>0.58</v>
       </c>
       <c r="B8" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D8" t="n">
         <v>486</v>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>Bob Doe</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="F8" t="n">
         <v>22</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
         <is>
           <t>Engineering</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>Morning</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr">
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
         <is>
           <t>£912-£1221</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="N8" t="inlineStr">
         <is>
           <t>UCL</t>
         </is>
@@ -841,47 +893,53 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.57</v>
+        <v>0.59</v>
       </c>
       <c r="B9" t="n">
-        <v>73</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Alice Smith</t>
-        </is>
+        <v>0.55</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-0.04</v>
       </c>
       <c r="D9" t="n">
-        <v>18</v>
+        <v>414</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Australia</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Cruising</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr">
+          <t>Alice Johnson</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>22</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>UK</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Computer Science</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
         <is>
           <t>Morning</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>£959-£1181</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>£631-£782</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
         <is>
           <t>UCL</t>
         </is>
@@ -892,48 +950,54 @@
         <v>0.52</v>
       </c>
       <c r="B10" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="D10" t="n">
         <v>404</v>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>Alice Smith</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="F10" t="n">
         <v>18</v>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>USA</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr">
         <is>
           <t>Business</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>Morning</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>£473-£686</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="N10" t="inlineStr">
         <is>
           <t>City</t>
         </is>
@@ -941,51 +1005,53 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.48</v>
+        <v>0.43</v>
       </c>
       <c r="B11" t="n">
-        <v>125</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Jane Smith</t>
-        </is>
+        <v>0.5</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.07000000000000001</v>
       </c>
       <c r="D11" t="n">
-        <v>22</v>
+        <v>430</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>USA</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Student</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr"/>
+          <t>Alice Smith</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>18</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Canada</t>
+        </is>
+      </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Computer Science</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>Morning</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
+          <t>Cruising</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Night</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>£707-£999</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>£394-£1948</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
         <is>
           <t>KCL</t>
         </is>
@@ -996,48 +1062,54 @@
         <v>0.46</v>
       </c>
       <c r="B12" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D12" t="n">
         <v>374</v>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>Jane Doe</t>
         </is>
       </c>
-      <c r="D12" t="n">
+      <c r="F12" t="n">
         <v>22</v>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr">
         <is>
           <t>Business</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="K12" t="inlineStr">
         <is>
           <t>Night</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="L12" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="M12" t="inlineStr">
         <is>
           <t>£780-£1075</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="N12" t="inlineStr">
         <is>
           <t>KCL</t>
         </is>
@@ -1045,47 +1117,57 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.43</v>
+        <v>0.48</v>
       </c>
       <c r="B13" t="n">
-        <v>430</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Alice Smith</t>
-        </is>
+        <v>0.46</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-0.02</v>
       </c>
       <c r="D13" t="n">
-        <v>18</v>
+        <v>125</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Cruising</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>Night</t>
-        </is>
-      </c>
+          <t>Jane Smith</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>22</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
+          <t>Computer Science</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
           <t>No</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>£394-£1948</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>£707-£999</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
         <is>
           <t>KCL</t>
         </is>
@@ -1096,48 +1178,50 @@
         <v>0.41</v>
       </c>
       <c r="B14" t="n">
-        <v>210</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Alice Doe</t>
-        </is>
+        <v>0.46</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.06</v>
       </c>
       <c r="D14" t="n">
+        <v>364</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Jane Doe</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
         <v>19</v>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>UK</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
         <is>
           <t>Working</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>Tech</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr">
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr">
         <is>
           <t>Night</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>£584-£1932</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>£700-£1713</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
         <is>
           <t>none</t>
         </is>
@@ -1148,44 +1232,54 @@
         <v>0.41</v>
       </c>
       <c r="B15" t="n">
-        <v>364</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Jane Doe</t>
-        </is>
+        <v>0.45</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.04</v>
       </c>
       <c r="D15" t="n">
+        <v>210</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Alice Doe</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
         <v>19</v>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>UK</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
         <is>
           <t>Working</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>Tech</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>Night</t>
         </is>
       </c>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr">
         <is>
-          <t>£700-£1713</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>£584-£1932</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
         <is>
           <t>none</t>
         </is>
@@ -1193,293 +1287,329 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.39</v>
+        <v>0.38</v>
       </c>
       <c r="B16" t="n">
-        <v>241</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>John Williams</t>
-        </is>
+        <v>0.45</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.06</v>
       </c>
       <c r="D16" t="n">
-        <v>22</v>
+        <v>279</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Australia</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Cruising</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
+          <t>Bob Williams</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>19</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Working</t>
+        </is>
+      </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Morning</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr">
         <is>
-          <t>£965-£1592</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>UCL</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>£643-£1855</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>QMU</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.39</v>
+        <v>0.36</v>
       </c>
       <c r="B17" t="n">
-        <v>370</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Alice Williams</t>
-        </is>
+        <v>0.42</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.06</v>
       </c>
       <c r="D17" t="n">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>UK</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Cruising</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
+          <t>Jane Doe</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>20</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Working</t>
+        </is>
+      </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Media</t>
         </is>
       </c>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr">
         <is>
-          <t>£552-£1046</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>UCL</t>
+          <t>Night</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>£812-£1801</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.38</v>
+        <v>0.39</v>
       </c>
       <c r="B18" t="n">
-        <v>279</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Bob Williams</t>
-        </is>
+        <v>0.42</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.03</v>
       </c>
       <c r="D18" t="n">
-        <v>19</v>
+        <v>370</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Working</t>
-        </is>
+          <t>Alice Williams</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>22</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>Night</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+          <t>UK</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Cruising</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr">
         <is>
-          <t>£643-£1855</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>QMU</t>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>£552-£1046</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>UCL</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.37</v>
+        <v>0.39</v>
       </c>
       <c r="B19" t="n">
-        <v>367</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Jane Smith</t>
-        </is>
+        <v>0.41</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.02</v>
       </c>
       <c r="D19" t="n">
+        <v>241</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>John Williams</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
         <v>22</v>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Student</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Engineering</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>Night</t>
-        </is>
-      </c>
+          <t>Cruising</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr">
         <is>
-          <t>£682-£924</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>KCL</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>£965-£1592</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>UCL</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.36</v>
+        <v>0.37</v>
       </c>
       <c r="B20" t="n">
-        <v>60</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Jane Doe</t>
-        </is>
+        <v>0.38</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.01</v>
       </c>
       <c r="D20" t="n">
-        <v>20</v>
+        <v>367</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
+          <t>Jane Smith</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>22</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
           <t>Australia</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Working</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Media</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr">
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
         <is>
           <t>Night</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>£812-£1801</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>none</t>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>£682-£924</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>KCL</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
       <c r="B21" t="n">
-        <v>479</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Jane Doe</t>
-        </is>
+        <v>0.33</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.02</v>
       </c>
       <c r="D21" t="n">
-        <v>22</v>
+        <v>285</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
+          <t>Bob Williams</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>21</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
           <t>UK</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Student</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Engineering</t>
+          <t>Working</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Night</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr">
         <is>
-          <t>£382-£533</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>City</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>£796-£1262</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>KCL</t>
         </is>
       </c>
     </row>
@@ -1488,300 +1618,340 @@
         <v>0.32</v>
       </c>
       <c r="B22" t="n">
-        <v>484</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Alice Smith</t>
-        </is>
+        <v>0.31</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-0.01</v>
       </c>
       <c r="D22" t="n">
-        <v>24</v>
+        <v>479</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>USA</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
+          <t>Jane Doe</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>22</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>UK</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>Computer Science</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>Morning</t>
-        </is>
-      </c>
+      <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>Engineering</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>£832-£1039</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>UCL</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>£382-£533</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>City</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.31</v>
+        <v>0.21</v>
       </c>
       <c r="B23" t="n">
-        <v>285</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Bob Williams</t>
-        </is>
+        <v>0.25</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.04</v>
       </c>
       <c r="D23" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>UK</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Working</t>
-        </is>
+          <t>Alice Williams</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>22</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr">
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Cruising</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr">
         <is>
           <t>Morning</t>
         </is>
       </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>£796-£1262</t>
-        </is>
-      </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>KCL</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>£357-£1605</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="B24" t="n">
-        <v>358</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>John Williams</t>
-        </is>
+        <v>0.25</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.02</v>
       </c>
       <c r="D24" t="n">
-        <v>26</v>
+        <v>296</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Australia</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Student</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr"/>
+          <t>Bob Williams</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>21</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Working</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Morning</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr">
         <is>
-          <t>£907-£1808</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>UCL</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>£772-£977</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>QMU</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.23</v>
+        <v>0.32</v>
       </c>
       <c r="B25" t="n">
-        <v>296</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Bob Williams</t>
-        </is>
+        <v>0.25</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-0.07000000000000001</v>
       </c>
       <c r="D25" t="n">
-        <v>21</v>
+        <v>484</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
+          <t>Alice Smith</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>24</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
           <t>USA</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Working</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>Night</t>
-        </is>
-      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr">
         <is>
+          <t>Computer Science</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>£772-£977</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>QMU</t>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>£832-£1039</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>UCL</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.21</v>
+        <v>0.24</v>
       </c>
       <c r="B26" t="n">
-        <v>19</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Alice Williams</t>
-        </is>
+        <v>0.19</v>
+      </c>
+      <c r="C26" t="n">
+        <v>-0.05</v>
       </c>
       <c r="D26" t="n">
-        <v>22</v>
+        <v>358</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
+          <t>John Williams</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>26</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
           <t>Australia</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Cruising</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr">
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Computer Science</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
         <is>
           <t>Morning</t>
         </is>
       </c>
-      <c r="J26" t="inlineStr">
+      <c r="L26" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>£357-£1605</t>
-        </is>
-      </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>none</t>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>£907-£1808</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>UCL</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="B27" t="n">
-        <v>47</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>John Williams</t>
-        </is>
+        <v>0.1</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-0.02</v>
       </c>
       <c r="D27" t="n">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>UK</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
+          <t>Jane Williams</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>25</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>Engineering</t>
-        </is>
-      </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>Morning</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Business</t>
+        </is>
+      </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>£773-£1082</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>£506-£1450</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
         <is>
           <t>UCL</t>
         </is>
@@ -1789,51 +1959,53 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="B28" t="n">
-        <v>58</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Jane Williams</t>
-        </is>
+        <v>0.1</v>
+      </c>
+      <c r="C28" t="n">
+        <v>-0.04</v>
       </c>
       <c r="D28" t="n">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Australia</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
+          <t>John Williams</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>26</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>UK</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>Business</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>Night</t>
-        </is>
-      </c>
+      <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Engineering</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>£506-£1450</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr">
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>£773-£1082</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
         <is>
           <t>UCL</t>
         </is>
@@ -1844,48 +2016,54 @@
         <v>0.08</v>
       </c>
       <c r="B29" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D29" t="n">
         <v>29</v>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>Bob Doe</t>
         </is>
       </c>
-      <c r="D29" t="n">
+      <c r="F29" t="n">
         <v>22</v>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="G29" t="inlineStr">
         <is>
           <t>Australia</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="H29" t="inlineStr">
         <is>
           <t>Working</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="I29" t="inlineStr">
         <is>
           <t>Finance</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr">
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr">
         <is>
           <t>Night</t>
         </is>
       </c>
-      <c r="J29" t="inlineStr">
+      <c r="L29" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="K29" t="inlineStr">
+      <c r="M29" t="inlineStr">
         <is>
           <t>£897-£901</t>
         </is>
       </c>
-      <c r="L29" t="inlineStr">
+      <c r="N29" t="inlineStr">
         <is>
           <t>City</t>
         </is>
@@ -1896,50 +2074,48 @@
         <v>0.03</v>
       </c>
       <c r="B30" t="n">
-        <v>224</v>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>John Johnson</t>
-        </is>
+        <v>0.05</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.02</v>
       </c>
       <c r="D30" t="n">
-        <v>24</v>
+        <v>490</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
+          <t>John Doe</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>23</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
           <t>Australia</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>Student</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Business</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr">
+          <t>Cruising</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr">
         <is>
           <t>Morning</t>
         </is>
       </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>£313-£1916</t>
-        </is>
-      </c>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>City</t>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>£733-£1615</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>KCL</t>
         </is>
       </c>
     </row>
@@ -1948,90 +2124,110 @@
         <v>0.03</v>
       </c>
       <c r="B31" t="n">
-        <v>490</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
+        <v>-0.01</v>
+      </c>
+      <c r="C31" t="n">
+        <v>-0.04</v>
       </c>
       <c r="D31" t="n">
-        <v>23</v>
+        <v>224</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
+          <t>John Johnson</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>24</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
           <t>Australia</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Cruising</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr">
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Business</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
         <is>
           <t>Morning</t>
         </is>
       </c>
-      <c r="J31" t="inlineStr"/>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>£733-£1615</t>
-        </is>
-      </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>KCL</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>£313-£1916</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>City</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
+        <v>-0.04</v>
+      </c>
+      <c r="B32" t="n">
         <v>-0.03</v>
       </c>
-      <c r="B32" t="n">
-        <v>223</v>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Jane Smith</t>
-        </is>
+      <c r="C32" t="n">
+        <v>0.01</v>
       </c>
       <c r="D32" t="n">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>UK</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Cruising</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
+          <t>John Doe</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>23</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Working</t>
+        </is>
+      </c>
       <c r="I32" t="inlineStr">
         <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr">
+        <is>
           <t>Morning</t>
         </is>
       </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>£666-£1444</t>
-        </is>
-      </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>UCL</t>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>£812-£1798</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>QMU</t>
         </is>
       </c>
     </row>
@@ -2040,90 +2236,110 @@
         <v>-0.04</v>
       </c>
       <c r="B33" t="n">
-        <v>317</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>John Johnson</t>
-        </is>
+        <v>-0.03</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.01</v>
       </c>
       <c r="D33" t="n">
+        <v>379</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Jane Johnson</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
         <v>23</v>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>Cruising</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Australia</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Working</t>
+        </is>
+      </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr">
         <is>
-          <t>£619-£928</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>KCL</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>£546-£1668</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="B34" t="n">
         <v>-0.04</v>
       </c>
-      <c r="B34" t="n">
-        <v>74</v>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
+      <c r="C34" t="n">
+        <v>-0.02</v>
       </c>
       <c r="D34" t="n">
-        <v>23</v>
+        <v>223</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>USA</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>Working</t>
-        </is>
+          <t>Jane Smith</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>24</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>Morning</t>
-        </is>
-      </c>
+          <t>UK</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Cruising</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr"/>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr">
         <is>
-          <t>£812-£1798</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>QMU</t>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>£666-£1444</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>UCL</t>
         </is>
       </c>
     </row>
@@ -2132,50 +2348,48 @@
         <v>-0.04</v>
       </c>
       <c r="B35" t="n">
-        <v>379</v>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Jane Johnson</t>
-        </is>
+        <v>-0.04</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0</v>
       </c>
       <c r="D35" t="n">
+        <v>317</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>John Johnson</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
         <v>23</v>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>Australia</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>Working</t>
-        </is>
-      </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Finance</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr">
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Cruising</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr">
         <is>
           <t>Morning</t>
         </is>
       </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>£546-£1668</t>
-        </is>
-      </c>
-      <c r="L35" t="inlineStr">
-        <is>
-          <t>none</t>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>£619-£928</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>KCL</t>
         </is>
       </c>
     </row>
@@ -2184,44 +2398,50 @@
         <v>-0.07000000000000001</v>
       </c>
       <c r="B36" t="n">
+        <v>-0.08</v>
+      </c>
+      <c r="C36" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="D36" t="n">
         <v>500</v>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="E36" t="inlineStr">
         <is>
           <t>Jane Doe</t>
         </is>
       </c>
-      <c r="D36" t="n">
+      <c r="F36" t="n">
         <v>26</v>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="G36" t="inlineStr">
         <is>
           <t>UK</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="H36" t="inlineStr">
         <is>
           <t>Cruising</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr">
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr">
         <is>
           <t>Night</t>
         </is>
       </c>
-      <c r="J36" t="inlineStr">
+      <c r="L36" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="K36" t="inlineStr">
+      <c r="M36" t="inlineStr">
         <is>
           <t>£345-£1268</t>
         </is>
       </c>
-      <c r="L36" t="inlineStr">
+      <c r="N36" t="inlineStr">
         <is>
           <t>UCL</t>
         </is>
@@ -2232,44 +2452,50 @@
         <v>-0.09</v>
       </c>
       <c r="B37" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="C37" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="D37" t="n">
         <v>301</v>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>Alice Williams</t>
         </is>
       </c>
-      <c r="D37" t="n">
+      <c r="F37" t="n">
         <v>23</v>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="G37" t="inlineStr">
         <is>
           <t>UK</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
+      <c r="H37" t="inlineStr">
         <is>
           <t>Working</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr">
+      <c r="I37" t="inlineStr">
         <is>
           <t>Tech</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>Morning</t>
         </is>
       </c>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr">
         <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr">
+        <is>
           <t>£916-£979</t>
         </is>
       </c>
-      <c r="L37" t="inlineStr">
+      <c r="N37" t="inlineStr">
         <is>
           <t>City</t>
         </is>
@@ -2277,101 +2503,113 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>-0.14</v>
+        <v>-0.17</v>
       </c>
       <c r="B38" t="n">
-        <v>203</v>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Jane Smith</t>
-        </is>
+        <v>-0.19</v>
+      </c>
+      <c r="C38" t="n">
+        <v>-0.02</v>
       </c>
       <c r="D38" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>UK</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>Student</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr"/>
+          <t>Alice Smith</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>24</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Canada</t>
+        </is>
+      </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Engineering</t>
-        </is>
-      </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>Morning</t>
-        </is>
-      </c>
-      <c r="J38" t="inlineStr">
+          <t>Cruising</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>Night</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>£307-£896</t>
-        </is>
-      </c>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>City</t>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>£993-£1261</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>QMU</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>-0.17</v>
+        <v>-0.14</v>
       </c>
       <c r="B39" t="n">
-        <v>16</v>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Alice Smith</t>
-        </is>
+        <v>-0.22</v>
+      </c>
+      <c r="C39" t="n">
+        <v>-0.09</v>
       </c>
       <c r="D39" t="n">
-        <v>24</v>
+        <v>203</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>Cruising</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="inlineStr"/>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>Night</t>
-        </is>
-      </c>
+          <t>Jane Smith</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>25</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>UK</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr"/>
       <c r="J39" t="inlineStr">
         <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>£993-£1261</t>
-        </is>
-      </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>QMU</t>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>£307-£896</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>City</t>
         </is>
       </c>
     </row>
@@ -2380,44 +2618,50 @@
         <v>-0.18</v>
       </c>
       <c r="B40" t="n">
+        <v>-0.24</v>
+      </c>
+      <c r="C40" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="D40" t="n">
         <v>435</v>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="E40" t="inlineStr">
         <is>
           <t>Alice Smith</t>
         </is>
       </c>
-      <c r="D40" t="n">
+      <c r="F40" t="n">
         <v>25</v>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="G40" t="inlineStr">
         <is>
           <t>Canada</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
+      <c r="H40" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr">
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr">
         <is>
           <t>Business</t>
         </is>
       </c>
-      <c r="I40" t="inlineStr">
+      <c r="K40" t="inlineStr">
         <is>
           <t>Morning</t>
         </is>
       </c>
-      <c r="J40" t="inlineStr"/>
-      <c r="K40" t="inlineStr">
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr">
         <is>
           <t>£671-£818</t>
         </is>
       </c>
-      <c r="L40" t="inlineStr">
+      <c r="N40" t="inlineStr">
         <is>
           <t>QMU</t>
         </is>
@@ -2428,48 +2672,54 @@
         <v>-0.24</v>
       </c>
       <c r="B41" t="n">
+        <v>-0.26</v>
+      </c>
+      <c r="C41" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="D41" t="n">
         <v>384</v>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="E41" t="inlineStr">
         <is>
           <t>Alice Johnson</t>
         </is>
       </c>
-      <c r="D41" t="n">
+      <c r="F41" t="n">
         <v>24</v>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="G41" t="inlineStr">
         <is>
           <t>UK</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr">
+      <c r="H41" t="inlineStr">
         <is>
           <t>Working</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr">
+      <c r="I41" t="inlineStr">
         <is>
           <t>Finance</t>
         </is>
       </c>
-      <c r="H41" t="inlineStr"/>
-      <c r="I41" t="inlineStr">
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr">
         <is>
           <t>Night</t>
         </is>
       </c>
-      <c r="J41" t="inlineStr">
+      <c r="L41" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="K41" t="inlineStr">
+      <c r="M41" t="inlineStr">
         <is>
           <t>£881-£1985</t>
         </is>
       </c>
-      <c r="L41" t="inlineStr">
+      <c r="N41" t="inlineStr">
         <is>
           <t>QMU</t>
         </is>
@@ -2477,101 +2727,113 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>-0.25</v>
+        <v>-0.26</v>
       </c>
       <c r="B42" t="n">
-        <v>50</v>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Bob Doe</t>
-        </is>
+        <v>-0.27</v>
+      </c>
+      <c r="C42" t="n">
+        <v>-0.01</v>
       </c>
       <c r="D42" t="n">
-        <v>24</v>
+        <v>135</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>UK</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>Working</t>
-        </is>
+          <t>Jane Doe</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>27</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Finance</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr"/>
-      <c r="I42" t="inlineStr">
+          <t>Canada</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Cruising</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr">
         <is>
           <t>Morning</t>
         </is>
       </c>
-      <c r="J42" t="inlineStr">
+      <c r="L42" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>£483-£1092</t>
-        </is>
-      </c>
-      <c r="L42" t="inlineStr">
-        <is>
-          <t>KCL</t>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>£674-£1257</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>City</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>-0.26</v>
+        <v>-0.25</v>
       </c>
       <c r="B43" t="n">
-        <v>135</v>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>Jane Doe</t>
-        </is>
+        <v>-0.28</v>
+      </c>
+      <c r="C43" t="n">
+        <v>-0.02</v>
       </c>
       <c r="D43" t="n">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>Cruising</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
+          <t>Bob Doe</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>24</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>UK</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Working</t>
+        </is>
+      </c>
       <c r="I43" t="inlineStr">
         <is>
+          <t>Finance</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr">
+        <is>
           <t>Morning</t>
         </is>
       </c>
-      <c r="J43" t="inlineStr">
+      <c r="L43" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>£674-£1257</t>
-        </is>
-      </c>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>City</t>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>£483-£1092</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>KCL</t>
         </is>
       </c>
     </row>
@@ -2580,48 +2842,54 @@
         <v>-0.29</v>
       </c>
       <c r="B44" t="n">
+        <v>-0.32</v>
+      </c>
+      <c r="C44" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="D44" t="n">
         <v>481</v>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="E44" t="inlineStr">
         <is>
           <t>Bob Smith</t>
         </is>
       </c>
-      <c r="D44" t="n">
+      <c r="F44" t="n">
         <v>26</v>
       </c>
-      <c r="E44" t="inlineStr">
+      <c r="G44" t="inlineStr">
         <is>
           <t>Canada</t>
         </is>
       </c>
-      <c r="F44" t="inlineStr">
+      <c r="H44" t="inlineStr">
         <is>
           <t>Working</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr">
+      <c r="I44" t="inlineStr">
         <is>
           <t>Media</t>
         </is>
       </c>
-      <c r="H44" t="inlineStr"/>
-      <c r="I44" t="inlineStr">
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr">
         <is>
           <t>Night</t>
         </is>
       </c>
-      <c r="J44" t="inlineStr">
+      <c r="L44" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K44" t="inlineStr">
+      <c r="M44" t="inlineStr">
         <is>
           <t>£936-£1935</t>
         </is>
       </c>
-      <c r="L44" t="inlineStr">
+      <c r="N44" t="inlineStr">
         <is>
           <t>QMU</t>
         </is>
@@ -2632,44 +2900,50 @@
         <v>-0.32</v>
       </c>
       <c r="B45" t="n">
+        <v>-0.35</v>
+      </c>
+      <c r="C45" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="D45" t="n">
         <v>411</v>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="E45" t="inlineStr">
         <is>
           <t>Jane Johnson</t>
         </is>
       </c>
-      <c r="D45" t="n">
+      <c r="F45" t="n">
         <v>25</v>
       </c>
-      <c r="E45" t="inlineStr">
+      <c r="G45" t="inlineStr">
         <is>
           <t>Canada</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr">
+      <c r="H45" t="inlineStr">
         <is>
           <t>Cruising</t>
         </is>
       </c>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr"/>
-      <c r="I45" t="inlineStr">
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr">
         <is>
           <t>Morning</t>
         </is>
       </c>
-      <c r="J45" t="inlineStr">
+      <c r="L45" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="K45" t="inlineStr">
+      <c r="M45" t="inlineStr">
         <is>
           <t>£335-£972</t>
         </is>
       </c>
-      <c r="L45" t="inlineStr">
+      <c r="N45" t="inlineStr">
         <is>
           <t>none</t>
         </is>
@@ -2680,48 +2954,54 @@
         <v>-0.34</v>
       </c>
       <c r="B46" t="n">
+        <v>-0.39</v>
+      </c>
+      <c r="C46" t="n">
+        <v>-0.06</v>
+      </c>
+      <c r="D46" t="n">
         <v>25</v>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="E46" t="inlineStr">
         <is>
           <t>Alice Smith</t>
         </is>
       </c>
-      <c r="D46" t="n">
+      <c r="F46" t="n">
         <v>27</v>
       </c>
-      <c r="E46" t="inlineStr">
+      <c r="G46" t="inlineStr">
         <is>
           <t>UK</t>
         </is>
       </c>
-      <c r="F46" t="inlineStr">
+      <c r="H46" t="inlineStr">
         <is>
           <t>Working</t>
         </is>
       </c>
-      <c r="G46" t="inlineStr">
+      <c r="I46" t="inlineStr">
         <is>
           <t>Tech</t>
         </is>
       </c>
-      <c r="H46" t="inlineStr"/>
-      <c r="I46" t="inlineStr">
+      <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr">
         <is>
           <t>Night</t>
         </is>
       </c>
-      <c r="J46" t="inlineStr">
+      <c r="L46" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K46" t="inlineStr">
+      <c r="M46" t="inlineStr">
         <is>
           <t>£596-£933</t>
         </is>
       </c>
-      <c r="L46" t="inlineStr">
+      <c r="N46" t="inlineStr">
         <is>
           <t>City</t>
         </is>
@@ -2732,44 +3012,50 @@
         <v>-0.38</v>
       </c>
       <c r="B47" t="n">
+        <v>-0.43</v>
+      </c>
+      <c r="C47" t="n">
+        <v>-0.05</v>
+      </c>
+      <c r="D47" t="n">
         <v>156</v>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="E47" t="inlineStr">
         <is>
           <t>John Johnson</t>
         </is>
       </c>
-      <c r="D47" t="n">
+      <c r="F47" t="n">
         <v>24</v>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="G47" t="inlineStr">
         <is>
           <t>UK</t>
         </is>
       </c>
-      <c r="F47" t="inlineStr">
+      <c r="H47" t="inlineStr">
         <is>
           <t>Working</t>
         </is>
       </c>
-      <c r="G47" t="inlineStr">
+      <c r="I47" t="inlineStr">
         <is>
           <t>Tech</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr"/>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>Night</t>
         </is>
       </c>
       <c r="J47" t="inlineStr"/>
       <c r="K47" t="inlineStr">
         <is>
+          <t>Night</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr">
+        <is>
           <t>£404-£571</t>
         </is>
       </c>
-      <c r="L47" t="inlineStr">
+      <c r="N47" t="inlineStr">
         <is>
           <t>QMU</t>
         </is>

</xml_diff>